<commit_message>
v1.0.19 corrección Excel threshold under 10
</commit_message>
<xml_diff>
--- a/Data/Parameters/Parámetros Revisión de Asientos Manuales de Compensación - Pruebas.xlsx
+++ b/Data/Parameters/Parámetros Revisión de Asientos Manuales de Compensación - Pruebas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S_RPA_CORP\Documents\UiPath\VOTOR-SOX-2024-002 Controles SOX-EAA-01.74.1-AR y SOX-EAA-02.74.1-AP y GL\Data\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9549201C-5909-472B-9697-BC622E56E1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD3BFE4-45CA-465F-8FAD-7DAB726656B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22890" windowHeight="10410" xr2:uid="{D9BD6469-DA06-4086-A45A-FED19CB1C737}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29010" windowHeight="13305" xr2:uid="{D9BD6469-DA06-4086-A45A-FED19CB1C737}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="2" r:id="rId1"/>
@@ -158,7 +158,7 @@
     <t>E002, E009, E026, E033, E061</t>
   </si>
   <si>
-    <t>lucy.serrano@vcimentos.com;jmruiz@rpatechnologies.es</t>
+    <t>jmruiz@rpatechnologies.es</t>
   </si>
 </sst>
 </file>

</xml_diff>